<commit_message>
ready to turn in
</commit_message>
<xml_diff>
--- a/ISYE 6501/Homework 3/Temps cusum.xlsx
+++ b/ISYE 6501/Homework 3/Temps cusum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8fbdb6882e83510/Documents/GitHub/omsa/ISYE 6501/Homework 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="348" documentId="8_{B4276107-7101-4EE2-BB6D-2665A993EA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F966E76-5FCD-40B1-99AE-E7186F35C8B8}"/>
+  <xr:revisionPtr revIDLastSave="349" documentId="8_{B4276107-7101-4EE2-BB6D-2665A993EA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D3CB10A-AB7A-4197-9606-F8F7BD7C3A5E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{3C407D5F-FCD6-43F6-8D6D-740F765737E7}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="6936" activeTab="1" xr2:uid="{3C407D5F-FCD6-43F6-8D6D-740F765737E7}"/>
   </bookViews>
   <sheets>
     <sheet name="temps raw" sheetId="2" r:id="rId1"/>
@@ -739,32 +739,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="31">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d;@"/>
+    </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1365,39 +1363,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d;@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -19227,7 +19207,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3670228B-A183-4C9B-866A-A1A049038E7B}" name="temps" displayName="temps" ref="A1:U124" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:U124" xr:uid="{3670228B-A183-4C9B-866A-A1A049038E7B}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{A1938B1C-B33B-4B7A-AC5B-AC093D1CDD40}" uniqueName="1" name="DAY" queryTableFieldId="1" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{A1938B1C-B33B-4B7A-AC5B-AC093D1CDD40}" uniqueName="1" name="DAY" queryTableFieldId="1" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{4E83F7D5-ADB9-4DCE-A973-5A5ED692D78E}" uniqueName="2" name="1996" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{2F9F068F-CB1B-45B9-8E0F-38E2796252F0}" uniqueName="3" name="1997" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{043FCE0F-58FB-4CBD-872D-226B0FF7F733}" uniqueName="4" name="1998" queryTableFieldId="4"/>
@@ -19257,7 +19237,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CA707AD7-4B7E-4FCF-8AA7-CC1D8247F4C5}" name="temps3" displayName="temps3" ref="A1:W125" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A1:W124" xr:uid="{3670228B-A183-4C9B-866A-A1A049038E7B}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{FE8141E9-75E1-49D9-8F9D-1D24DFB7FEE7}" uniqueName="1" name="DAY" queryTableFieldId="1" dataDxfId="31" totalsRowDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{FE8141E9-75E1-49D9-8F9D-1D24DFB7FEE7}" uniqueName="1" name="DAY" queryTableFieldId="1" dataDxfId="29" totalsRowDxfId="1"/>
     <tableColumn id="2" xr3:uid="{3933BDDF-4052-4260-ACEF-2D16ABF57267}" uniqueName="2" name="1996" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{49688B52-C43F-4275-AF8D-5B842FB9E661}" uniqueName="3" name="1997" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{6C0503FC-3445-453F-9E62-F16A9F92A26B}" uniqueName="4" name="1998" queryTableFieldId="4"/>
@@ -19278,7 +19258,7 @@
     <tableColumn id="19" xr3:uid="{D575949A-4853-486B-B249-D93A948AAEAC}" uniqueName="19" name="2013" queryTableFieldId="19"/>
     <tableColumn id="20" xr3:uid="{917C7F07-36A8-4C9B-8018-04B40BAC8966}" uniqueName="20" name="2014" totalsRowLabel="50" queryTableFieldId="20"/>
     <tableColumn id="21" xr3:uid="{8E0ED615-ACC6-404C-B1D9-C4B0515549D5}" uniqueName="21" name="2015" totalsRowLabel="105" queryTableFieldId="21"/>
-    <tableColumn id="22" xr3:uid="{DD0186C4-4A9E-42F3-A591-20576065A4CC}" uniqueName="22" name="Avg" totalsRowLabel="83.34" queryTableFieldId="22" dataDxfId="30" totalsRowDxfId="24"/>
+    <tableColumn id="22" xr3:uid="{DD0186C4-4A9E-42F3-A591-20576065A4CC}" uniqueName="22" name="Avg" totalsRowLabel="83.34" queryTableFieldId="22" dataDxfId="28" totalsRowDxfId="0"/>
     <tableColumn id="23" xr3:uid="{BF5D7834-E86D-4A9E-B015-3627F9F0E7FB}" uniqueName="23" name="Detected" queryTableFieldId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -19289,38 +19269,38 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{190AD61C-3B01-4059-89A9-8B2D1C9F3594}" name="temps34" displayName="temps34" ref="A1:B5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B5" xr:uid="{3670228B-A183-4C9B-866A-A1A049038E7B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{77BEF03A-A91A-4336-BF6E-FEBB136DE09D}" uniqueName="1" name="DAY" queryTableFieldId="1" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="22" xr3:uid="{BE460F1B-CAD2-4D92-9FEA-B5645A4315C8}" uniqueName="22" name="Avg" queryTableFieldId="22" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{77BEF03A-A91A-4336-BF6E-FEBB136DE09D}" uniqueName="1" name="DAY" queryTableFieldId="1" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="22" xr3:uid="{BE460F1B-CAD2-4D92-9FEA-B5645A4315C8}" uniqueName="22" name="Avg" queryTableFieldId="22" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{72DD4E19-C422-47CC-A9BE-D253ABE39972}" name="Table4" displayName="Table4" ref="A24:U25" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{72DD4E19-C422-47CC-A9BE-D253ABE39972}" name="Table4" displayName="Table4" ref="A24:U25" totalsRowShown="0" dataDxfId="24">
   <autoFilter ref="A24:U25" xr:uid="{72DD4E19-C422-47CC-A9BE-D253ABE39972}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{1228A036-B220-479F-B808-7411F0FD5FC6}" name="DAY" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{9828A485-2803-4F29-A8E8-38AC224460EE}" name="1996" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{A6E6D037-B4B6-42DF-9688-9C82FD1EE077}" name="1997" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{7B6E55A5-927D-4C72-BB51-A4E1B49C03FA}" name="1998" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{EDB0B01F-382A-4E17-BD2A-201165D56AAF}" name="1999" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{A2694844-A868-4412-BA4E-ADD080AE8DCB}" name="2000" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{B3FC6B2C-5E60-4B61-A8AC-4BA26CCE356B}" name="2001" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{4C724FC1-F890-497D-991E-8D9D648FF149}" name="2002" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{45F35464-C37D-48C2-896C-B564202EC701}" name="2003" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{1A8F07B2-1492-4B3F-80F5-EDEC240262F8}" name="2004" dataDxfId="12"/>
-    <tableColumn id="11" xr3:uid="{C26B1FEC-7432-46DB-B1A0-64D6EAC9423E}" name="2005" dataDxfId="11"/>
-    <tableColumn id="12" xr3:uid="{D0D0B655-3CB1-4F81-8CFD-56D0C312F137}" name="2006" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{CB6263F1-E03B-417D-9A4D-9236D74E41FE}" name="2007" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{C3E0F34A-A4F6-4724-899B-A6512E04595B}" name="2008" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{CB516417-275F-42D5-A09D-62D03E607C11}" name="2009" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{39A01121-A813-49E7-8596-04DA19073E2B}" name="2010" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{284CC5C0-4CD1-4BB1-B07C-6D849966CFA4}" name="2011" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{62D28207-3D4F-4EA8-A433-327899396258}" name="2012" dataDxfId="4"/>
-    <tableColumn id="19" xr3:uid="{BD1D73BA-AF3D-4F48-89C2-5170C991F3D4}" name="2013" dataDxfId="3"/>
-    <tableColumn id="20" xr3:uid="{C1AA8F04-58CA-493F-9398-436AD163397B}" name="2014" dataDxfId="2"/>
-    <tableColumn id="21" xr3:uid="{B3FD13B0-DFF7-4F81-9A0C-14C1E45C4DC3}" name="2015" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{1228A036-B220-479F-B808-7411F0FD5FC6}" name="DAY" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{9828A485-2803-4F29-A8E8-38AC224460EE}" name="1996" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{A6E6D037-B4B6-42DF-9688-9C82FD1EE077}" name="1997" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{7B6E55A5-927D-4C72-BB51-A4E1B49C03FA}" name="1998" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{EDB0B01F-382A-4E17-BD2A-201165D56AAF}" name="1999" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{A2694844-A868-4412-BA4E-ADD080AE8DCB}" name="2000" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{B3FC6B2C-5E60-4B61-A8AC-4BA26CCE356B}" name="2001" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{4C724FC1-F890-497D-991E-8D9D648FF149}" name="2002" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{45F35464-C37D-48C2-896C-B564202EC701}" name="2003" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{1A8F07B2-1492-4B3F-80F5-EDEC240262F8}" name="2004" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{C26B1FEC-7432-46DB-B1A0-64D6EAC9423E}" name="2005" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{D0D0B655-3CB1-4F81-8CFD-56D0C312F137}" name="2006" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{CB6263F1-E03B-417D-9A4D-9236D74E41FE}" name="2007" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{C3E0F34A-A4F6-4724-899B-A6512E04595B}" name="2008" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{CB516417-275F-42D5-A09D-62D03E607C11}" name="2009" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{39A01121-A813-49E7-8596-04DA19073E2B}" name="2010" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{284CC5C0-4CD1-4BB1-B07C-6D849966CFA4}" name="2011" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{62D28207-3D4F-4EA8-A433-327899396258}" name="2012" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{BD1D73BA-AF3D-4F48-89C2-5170C991F3D4}" name="2013" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{C1AA8F04-58CA-493F-9398-436AD163397B}" name="2014" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{B3FD13B0-DFF7-4F81-9A0C-14C1E45C4DC3}" name="2015" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -19645,15 +19625,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25CDA41-6510-457D-9ED1-A37AD9FE3B97}">
   <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView showFormulas="1" workbookViewId="0"/>
+    <sheetView showFormulas="1" topLeftCell="N1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="21" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -19718,7 +19698,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -19783,7 +19763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -19848,7 +19828,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -19913,7 +19893,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -19978,7 +19958,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -20043,7 +20023,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -20108,7 +20088,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -20173,7 +20153,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -20238,7 +20218,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -20303,7 +20283,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -20368,7 +20348,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -20433,7 +20413,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -20498,7 +20478,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -20563,7 +20543,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -20628,7 +20608,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -20693,7 +20673,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -20758,7 +20738,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -20823,7 +20803,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -20888,7 +20868,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -20953,7 +20933,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -21018,7 +20998,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -21083,7 +21063,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -21148,7 +21128,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -21213,7 +21193,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -21278,7 +21258,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -21343,7 +21323,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -21408,7 +21388,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -21473,7 +21453,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -21538,7 +21518,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -21603,7 +21583,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -21668,7 +21648,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -21733,7 +21713,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -21798,7 +21778,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -21863,7 +21843,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -21928,7 +21908,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -21993,7 +21973,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -22058,7 +22038,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -22123,7 +22103,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -22188,7 +22168,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -22253,7 +22233,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -22318,7 +22298,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -22383,7 +22363,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -22448,7 +22428,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -22513,7 +22493,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -22578,7 +22558,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -22643,7 +22623,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -22708,7 +22688,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -22773,7 +22753,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -22838,7 +22818,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -22903,7 +22883,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -22968,7 +22948,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -23033,7 +23013,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -23098,7 +23078,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -23163,7 +23143,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -23228,7 +23208,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -23293,7 +23273,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -23358,7 +23338,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -23423,7 +23403,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -23488,7 +23468,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -23553,7 +23533,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -23618,7 +23598,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -23683,7 +23663,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -23748,7 +23728,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -23813,7 +23793,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -23878,7 +23858,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -23943,7 +23923,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -24008,7 +23988,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -24073,7 +24053,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -24138,7 +24118,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -24203,7 +24183,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -24268,7 +24248,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -24333,7 +24313,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -24398,7 +24378,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -24463,7 +24443,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -24528,7 +24508,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -24593,7 +24573,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -24658,7 +24638,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -24723,7 +24703,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -24788,7 +24768,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -24853,7 +24833,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -24918,7 +24898,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -24983,7 +24963,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -25048,7 +25028,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -25113,7 +25093,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -25178,7 +25158,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -25243,7 +25223,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -25308,7 +25288,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -25373,7 +25353,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -25438,7 +25418,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -25503,7 +25483,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -25568,7 +25548,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -25633,7 +25613,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -25698,7 +25678,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -25763,7 +25743,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -25828,7 +25808,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -25893,7 +25873,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -25958,7 +25938,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -26023,7 +26003,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -26088,7 +26068,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -26153,7 +26133,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -26218,7 +26198,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -26283,7 +26263,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -26348,7 +26328,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -26413,7 +26393,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -26478,7 +26458,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -26543,7 +26523,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -26608,7 +26588,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -26673,7 +26653,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -26738,7 +26718,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -26803,7 +26783,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -26868,7 +26848,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -26933,7 +26913,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -26998,7 +26978,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -27063,7 +27043,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -27128,7 +27108,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -27193,7 +27173,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -27258,7 +27238,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -27323,7 +27303,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -27388,7 +27368,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -27453,7 +27433,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -27518,7 +27498,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -27583,7 +27563,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -27648,7 +27628,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -27725,16 +27705,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A43C642-966E-4796-8040-1099A304EA2D}">
   <dimension ref="A1:AC129"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -27820,7 +27802,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -27906,7 +27888,7 @@
         <v>83.75</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -27985,7 +27967,7 @@
         <v>83.75</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -28053,7 +28035,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -28121,7 +28103,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -28189,7 +28171,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -28257,7 +28239,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -28325,7 +28307,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
@@ -28393,7 +28375,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -28461,7 +28443,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -28529,7 +28511,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -28597,7 +28579,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
@@ -28665,7 +28647,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -28733,7 +28715,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
@@ -28801,7 +28783,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
@@ -28869,7 +28851,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>16</v>
       </c>
@@ -28937,7 +28919,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -29005,7 +28987,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -29073,7 +29055,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -29141,7 +29123,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -29209,7 +29191,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>21</v>
       </c>
@@ -29277,7 +29259,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>22</v>
       </c>
@@ -29345,7 +29327,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>23</v>
       </c>
@@ -29413,7 +29395,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>24</v>
       </c>
@@ -29481,7 +29463,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>25</v>
       </c>
@@ -29549,7 +29531,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
@@ -29617,7 +29599,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
@@ -29685,7 +29667,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>28</v>
       </c>
@@ -29753,7 +29735,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
@@ -29821,7 +29803,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -29889,7 +29871,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>31</v>
       </c>
@@ -29957,7 +29939,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
@@ -30025,7 +30007,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>33</v>
       </c>
@@ -30093,7 +30075,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>34</v>
       </c>
@@ -30161,7 +30143,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>35</v>
       </c>
@@ -30229,7 +30211,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>36</v>
       </c>
@@ -30297,7 +30279,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>37</v>
       </c>
@@ -30365,7 +30347,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>38</v>
       </c>
@@ -30433,7 +30415,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>39</v>
       </c>
@@ -30501,7 +30483,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>40</v>
       </c>
@@ -30569,7 +30551,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>41</v>
       </c>
@@ -30637,7 +30619,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>42</v>
       </c>
@@ -30705,7 +30687,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>43</v>
       </c>
@@ -30773,7 +30755,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>44</v>
       </c>
@@ -30841,7 +30823,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>45</v>
       </c>
@@ -30909,7 +30891,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>46</v>
       </c>
@@ -30977,7 +30959,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>47</v>
       </c>
@@ -31045,7 +31027,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>48</v>
       </c>
@@ -31113,7 +31095,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>49</v>
       </c>
@@ -31181,7 +31163,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>50</v>
       </c>
@@ -31249,7 +31231,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>51</v>
       </c>
@@ -31317,7 +31299,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>52</v>
       </c>
@@ -31385,7 +31367,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>53</v>
       </c>
@@ -31453,7 +31435,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>54</v>
       </c>
@@ -31521,7 +31503,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>55</v>
       </c>
@@ -31589,7 +31571,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>56</v>
       </c>
@@ -31657,7 +31639,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>57</v>
       </c>
@@ -31725,7 +31707,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>58</v>
       </c>
@@ -31793,7 +31775,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>59</v>
       </c>
@@ -31861,7 +31843,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>60</v>
       </c>
@@ -31929,7 +31911,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>61</v>
       </c>
@@ -31997,7 +31979,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>62</v>
       </c>
@@ -32065,7 +32047,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>63</v>
       </c>
@@ -32133,7 +32115,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>64</v>
       </c>
@@ -32201,7 +32183,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>65</v>
       </c>
@@ -32269,7 +32251,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>66</v>
       </c>
@@ -32337,7 +32319,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>67</v>
       </c>
@@ -32405,7 +32387,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>68</v>
       </c>
@@ -32473,7 +32455,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>69</v>
       </c>
@@ -32541,7 +32523,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>70</v>
       </c>
@@ -32609,7 +32591,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>71</v>
       </c>
@@ -32677,7 +32659,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>72</v>
       </c>
@@ -32745,7 +32727,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>73</v>
       </c>
@@ -32813,7 +32795,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>74</v>
       </c>
@@ -32881,7 +32863,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>75</v>
       </c>
@@ -32949,7 +32931,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>76</v>
       </c>
@@ -33017,7 +32999,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>77</v>
       </c>
@@ -33085,7 +33067,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>78</v>
       </c>
@@ -33153,7 +33135,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>79</v>
       </c>
@@ -33221,7 +33203,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>80</v>
       </c>
@@ -33289,7 +33271,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>81</v>
       </c>
@@ -33357,7 +33339,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>82</v>
       </c>
@@ -33425,7 +33407,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>83</v>
       </c>
@@ -33493,7 +33475,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>84</v>
       </c>
@@ -33561,7 +33543,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>85</v>
       </c>
@@ -33629,7 +33611,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>86</v>
       </c>
@@ -33697,7 +33679,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>87</v>
       </c>
@@ -33765,7 +33747,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>88</v>
       </c>
@@ -33833,7 +33815,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>89</v>
       </c>
@@ -33901,7 +33883,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>90</v>
       </c>
@@ -33969,7 +33951,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>91</v>
       </c>
@@ -34037,7 +34019,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>92</v>
       </c>
@@ -34105,7 +34087,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>93</v>
       </c>
@@ -34173,7 +34155,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>94</v>
       </c>
@@ -34241,7 +34223,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>95</v>
       </c>
@@ -34309,7 +34291,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>96</v>
       </c>
@@ -34377,7 +34359,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>97</v>
       </c>
@@ -34445,7 +34427,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>98</v>
       </c>
@@ -34513,7 +34495,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>99</v>
       </c>
@@ -34581,7 +34563,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>100</v>
       </c>
@@ -34649,7 +34631,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>101</v>
       </c>
@@ -34717,7 +34699,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>102</v>
       </c>
@@ -34785,7 +34767,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>103</v>
       </c>
@@ -34853,7 +34835,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>104</v>
       </c>
@@ -34921,7 +34903,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>105</v>
       </c>
@@ -34989,7 +34971,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>106</v>
       </c>
@@ -35057,7 +35039,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>107</v>
       </c>
@@ -35125,7 +35107,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>108</v>
       </c>
@@ -35193,7 +35175,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>109</v>
       </c>
@@ -35261,7 +35243,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>110</v>
       </c>
@@ -35329,7 +35311,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>111</v>
       </c>
@@ -35397,7 +35379,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>112</v>
       </c>
@@ -35465,7 +35447,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>113</v>
       </c>
@@ -35533,7 +35515,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>114</v>
       </c>
@@ -35601,7 +35583,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>115</v>
       </c>
@@ -35669,7 +35651,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>116</v>
       </c>
@@ -35737,7 +35719,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>117</v>
       </c>
@@ -35805,7 +35787,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>118</v>
       </c>
@@ -35873,7 +35855,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>119</v>
       </c>
@@ -35941,7 +35923,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>120</v>
       </c>
@@ -36009,7 +35991,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>121</v>
       </c>
@@ -36077,7 +36059,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>122</v>
       </c>
@@ -36145,7 +36127,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>123</v>
       </c>
@@ -36213,7 +36195,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A125" s="1"/>
       <c r="T125" t="s">
         <v>157</v>
@@ -36225,7 +36207,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.3">
       <c r="T126" t="s">
         <v>147</v>
       </c>
@@ -36236,18 +36218,18 @@
         <v>145</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.3">
       <c r="V127" s="2"/>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.3">
       <c r="V128" s="2"/>
     </row>
-    <row r="129" spans="22:22" x14ac:dyDescent="0.25">
+    <row r="129" spans="22:22" x14ac:dyDescent="0.3">
       <c r="V129" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:V124">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>$AB$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36290,20 +36272,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700E34D0-A0EA-466D-84CC-CF3125F2A35F}">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36311,7 +36293,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>151</v>
       </c>
@@ -36319,7 +36301,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>148</v>
       </c>
@@ -36327,7 +36309,7 @@
         <v>88.616129032258058</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>149</v>
       </c>
@@ -36335,7 +36317,7 @@
         <v>82.671666666666667</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>150</v>
       </c>
@@ -36343,19 +36325,19 @@
         <v>73.296774193548387</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -36420,7 +36402,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>84</v>
       </c>

</xml_diff>